<commit_message>
pydentify got deleted somehow. reverted to pydentify from 6497b5a9ea80fca3525d45d0fdf04ec39b7158ec
</commit_message>
<xml_diff>
--- a/PyCoTools/PyCoToolsTutorial/Test/PEConfigFile.xlsx
+++ b/PyCoTools/PyCoToolsTutorial/Test/PEConfigFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="116">
   <si>
     <t>start_value</t>
   </si>
@@ -67,9 +67,6 @@
     <t>(TestREaction).k1</t>
   </si>
   <si>
-    <t>(TestREaction).k2</t>
-  </si>
-  <si>
     <t>(dephosphorylation of MAPKK-PP).KK5</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
     <t>(MAPKKK activation).n</t>
   </si>
   <si>
+    <t>test_globl</t>
+  </si>
+  <si>
     <t>Mek1-PP</t>
   </si>
   <si>
@@ -139,49 +139,106 @@
     <t>Mek1-P</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.025</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>9.99999845072</t>
-  </si>
-  <si>
-    <t>0.999999845072</t>
-  </si>
-  <si>
-    <t>279.99995662</t>
-  </si>
-  <si>
-    <t>89.9999860565</t>
+    <t>153697</t>
+  </si>
+  <si>
+    <t>1.55654e-06</t>
+  </si>
+  <si>
+    <t>91.2283</t>
+  </si>
+  <si>
+    <t>0.00454959</t>
+  </si>
+  <si>
+    <t>5.47613</t>
+  </si>
+  <si>
+    <t>0.06989090000000001</t>
+  </si>
+  <si>
+    <t>4904.34</t>
+  </si>
+  <si>
+    <t>116.058</t>
+  </si>
+  <si>
+    <t>15.6609</t>
+  </si>
+  <si>
+    <t>968526</t>
+  </si>
+  <si>
+    <t>1.05986e-06</t>
+  </si>
+  <si>
+    <t>44.8609</t>
+  </si>
+  <si>
+    <t>3288.05</t>
+  </si>
+  <si>
+    <t>1.0539e-06</t>
+  </si>
+  <si>
+    <t>2.95684</t>
+  </si>
+  <si>
+    <t>0.06533750000000001</t>
+  </si>
+  <si>
+    <t>367.525</t>
+  </si>
+  <si>
+    <t>6.68402e-06</t>
+  </si>
+  <si>
+    <t>1.83009e-06</t>
+  </si>
+  <si>
+    <t>0.0735201</t>
+  </si>
+  <si>
+    <t>8.957479999999999e-05</t>
+  </si>
+  <si>
+    <t>0.0103187</t>
+  </si>
+  <si>
+    <t>34678.2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1.05345e-05</t>
+  </si>
+  <si>
+    <t>0.00310584999982</t>
+  </si>
+  <si>
+    <t>7.07079e-06</t>
+  </si>
+  <si>
+    <t>0.00128073</t>
+  </si>
+  <si>
+    <t>2.5475e-06</t>
+  </si>
+  <si>
+    <t>8.89916e-06</t>
+  </si>
+  <si>
+    <t>7.35755</t>
+  </si>
+  <si>
+    <t>1.24798e-06</t>
+  </si>
+  <si>
+    <t>9.22585e-05</t>
+  </si>
+  <si>
+    <t>0.00447167</t>
   </si>
   <si>
     <t>1e-06</t>
@@ -199,6 +256,9 @@
     <t>ReactionParameter</t>
   </si>
   <si>
+    <t>ModelValue</t>
+  </si>
+  <si>
     <t>Species</t>
   </si>
   <si>
@@ -232,9 +292,6 @@
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[TestREaction],ParameterGroup=Parameters,Parameter=k1</t>
   </si>
   <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[TestREaction],ParameterGroup=Parameters,Parameter=k2</t>
-  </si>
-  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-PP],ParameterGroup=Parameters,Parameter=KK5</t>
   </si>
   <si>
@@ -272,6 +329,9 @@
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=n</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Values[test_globl]</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Compartments[uVol],Vector=Metabolites[Mek1-PP]</t>
@@ -696,19 +756,19 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -719,19 +779,19 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -742,19 +802,19 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -765,19 +825,19 @@
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -785,22 +845,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -808,22 +868,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -831,22 +891,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -854,22 +914,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -877,22 +937,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -900,22 +960,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -923,22 +983,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -946,22 +1006,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -969,22 +1029,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -992,22 +1052,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1015,22 +1075,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1038,22 +1098,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1061,22 +1121,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1084,22 +1144,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1107,22 +1167,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1130,22 +1190,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1153,22 +1213,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1176,22 +1236,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1199,22 +1259,22 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1222,22 +1282,22 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1245,22 +1305,22 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1268,22 +1328,22 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1291,22 +1351,22 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1314,22 +1374,22 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1337,22 +1397,22 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1360,22 +1420,22 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1383,22 +1443,22 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1406,22 +1466,22 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1429,22 +1489,22 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1452,22 +1512,22 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G35" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pydentify got deleted somehow. reverted to pydentify from f0776570b019fc02682154dc226434c1759e246f
</commit_message>
<xml_diff>
--- a/PyCoTools/PyCoToolsTutorial/Test/PEConfigFile.xlsx
+++ b/PyCoTools/PyCoToolsTutorial/Test/PEConfigFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="116">
   <si>
     <t>start_value</t>
   </si>
@@ -67,9 +67,6 @@
     <t>(TestREaction).k1</t>
   </si>
   <si>
-    <t>(TestREaction).k2</t>
-  </si>
-  <si>
     <t>(dephosphorylation of MAPKK-PP).KK5</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
     <t>(MAPKKK activation).n</t>
   </si>
   <si>
+    <t>test_globl</t>
+  </si>
+  <si>
     <t>Mek1-PP</t>
   </si>
   <si>
@@ -139,49 +139,106 @@
     <t>Mek1-P</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.025</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>9.99999845072</t>
-  </si>
-  <si>
-    <t>0.999999845072</t>
-  </si>
-  <si>
-    <t>279.99995662</t>
-  </si>
-  <si>
-    <t>89.9999860565</t>
+    <t>153697</t>
+  </si>
+  <si>
+    <t>1.55654e-06</t>
+  </si>
+  <si>
+    <t>91.2283</t>
+  </si>
+  <si>
+    <t>0.00454959</t>
+  </si>
+  <si>
+    <t>5.47613</t>
+  </si>
+  <si>
+    <t>0.06989090000000001</t>
+  </si>
+  <si>
+    <t>4904.34</t>
+  </si>
+  <si>
+    <t>116.058</t>
+  </si>
+  <si>
+    <t>15.6609</t>
+  </si>
+  <si>
+    <t>968526</t>
+  </si>
+  <si>
+    <t>1.05986e-06</t>
+  </si>
+  <si>
+    <t>44.8609</t>
+  </si>
+  <si>
+    <t>3288.05</t>
+  </si>
+  <si>
+    <t>1.0539e-06</t>
+  </si>
+  <si>
+    <t>2.95684</t>
+  </si>
+  <si>
+    <t>0.06533750000000001</t>
+  </si>
+  <si>
+    <t>367.525</t>
+  </si>
+  <si>
+    <t>6.68402e-06</t>
+  </si>
+  <si>
+    <t>1.83009e-06</t>
+  </si>
+  <si>
+    <t>0.0735201</t>
+  </si>
+  <si>
+    <t>8.957479999999999e-05</t>
+  </si>
+  <si>
+    <t>0.0103187</t>
+  </si>
+  <si>
+    <t>34678.2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1.05345e-05</t>
+  </si>
+  <si>
+    <t>0.00310584999982</t>
+  </si>
+  <si>
+    <t>7.07079e-06</t>
+  </si>
+  <si>
+    <t>0.00128073</t>
+  </si>
+  <si>
+    <t>2.5475e-06</t>
+  </si>
+  <si>
+    <t>8.89916e-06</t>
+  </si>
+  <si>
+    <t>7.35755</t>
+  </si>
+  <si>
+    <t>1.24798e-06</t>
+  </si>
+  <si>
+    <t>9.22585e-05</t>
+  </si>
+  <si>
+    <t>0.00447167</t>
   </si>
   <si>
     <t>1e-06</t>
@@ -199,6 +256,9 @@
     <t>ReactionParameter</t>
   </si>
   <si>
+    <t>ModelValue</t>
+  </si>
+  <si>
     <t>Species</t>
   </si>
   <si>
@@ -232,9 +292,6 @@
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[TestREaction],ParameterGroup=Parameters,Parameter=k1</t>
   </si>
   <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[TestREaction],ParameterGroup=Parameters,Parameter=k2</t>
-  </si>
-  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-PP],ParameterGroup=Parameters,Parameter=KK5</t>
   </si>
   <si>
@@ -272,6 +329,9 @@
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=n</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Values[test_globl]</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Compartments[uVol],Vector=Metabolites[Mek1-PP]</t>
@@ -696,19 +756,19 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -719,19 +779,19 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -742,19 +802,19 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -765,19 +825,19 @@
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -785,22 +845,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -808,22 +868,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -831,22 +891,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -854,22 +914,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -877,22 +937,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -900,22 +960,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -923,22 +983,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -946,22 +1006,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -969,22 +1029,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -992,22 +1052,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1015,22 +1075,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1038,22 +1098,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1061,22 +1121,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1084,22 +1144,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1107,22 +1167,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1130,22 +1190,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1153,22 +1213,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1176,22 +1236,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1199,22 +1259,22 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1222,22 +1282,22 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1245,22 +1305,22 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1268,22 +1328,22 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1291,22 +1351,22 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1314,22 +1374,22 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1337,22 +1397,22 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1360,22 +1420,22 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1383,22 +1443,22 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1406,22 +1466,22 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1429,22 +1489,22 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1452,22 +1512,22 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="G35" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>